<commit_message>
Implemented Bayesian Optimization for XGBoost. In process to implement for CatBoost and Sklearn. Updated AWS scripts to be flexible regardless of the API used. Updated RealEstate class to be flexible regardless of API used.
</commit_message>
<xml_diff>
--- a/docs/Model Histories.xlsx
+++ b/docs/Model Histories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\Real_Estate_Analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B4C5F51-EC3D-40A1-967D-456F2705C7F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E021000-FF99-4CAE-8D01-BB03696FFE9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20616" yWindow="2232" windowWidth="19176" windowHeight="11856" xr2:uid="{A6735569-3412-48D9-A81F-E34E4DFEE9CE}"/>
+    <workbookView xWindow="11544" yWindow="2232" windowWidth="19176" windowHeight="11856" xr2:uid="{A6735569-3412-48D9-A81F-E34E4DFEE9CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Deep Learning Model</t>
   </si>
@@ -54,15 +54,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Sklearn</t>
-  </si>
-  <si>
-    <t>AWS Sagemaker - Raw</t>
-  </si>
-  <si>
-    <t>AWS Sagemaker - Encoded</t>
   </si>
   <si>
     <t>Best vs Worst Performance</t>
@@ -169,6 +160,12 @@
   </si>
   <si>
     <t>Reduction in training time between Bayesian Optimization and Incremental Grid Search</t>
+  </si>
+  <si>
+    <t>BO XGBOOST w/o Tags</t>
+  </si>
+  <si>
+    <t>BO XGBOOST Sold</t>
   </si>
 </sst>
 </file>
@@ -178,10 +175,10 @@
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="0.000%"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -244,15 +241,15 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -262,13 +259,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -279,25 +276,25 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000"/>
+      <numFmt numFmtId="166" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000"/>
+      <numFmt numFmtId="166" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000"/>
+      <numFmt numFmtId="166" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -332,30 +329,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{199E95C3-890B-4BD6-89DF-E2E7224A9CDD}" name="Table1" displayName="Table1" ref="A9:J13" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{199E95C3-890B-4BD6-89DF-E2E7224A9CDD}" name="Table1" displayName="Table1" ref="A9:J13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A9:J13" xr:uid="{B00E93C4-8508-4C88-BAE2-DE0BA5DD3185}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F0D93059-BE22-486E-B143-D32310CD21F5}" name="Method" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7483B5A0-2D20-4415-8D69-7852762BB1F5}" name="Models" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{F0D93059-BE22-486E-B143-D32310CD21F5}" name="Method" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{7483B5A0-2D20-4415-8D69-7852762BB1F5}" name="Models" dataDxfId="8">
       <calculatedColumnFormula>3^8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D2A2F514-96D0-48DA-B585-9712F22A0880}" name="Total Tasks" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{D2A2F514-96D0-48DA-B585-9712F22A0880}" name="Total Tasks" dataDxfId="7">
       <calculatedColumnFormula>B10*5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{20D93D46-EA4C-46CD-9954-6489D16856AA}" name="Total Time (s)" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{20D93D46-EA4C-46CD-9954-6489D16856AA}" name="Total Time (s)" dataDxfId="6">
       <calculatedColumnFormula>C10*#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{40716B2A-D642-4BD7-AB28-612299D1634E}" name="Total Time (min)" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{40716B2A-D642-4BD7-AB28-612299D1634E}" name="Total Time (min)" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[Total Time (s)]]/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5498A1F2-53C7-4B44-9245-0B42822822E1}" name="Total Time (hours)" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{5498A1F2-53C7-4B44-9245-0B42822822E1}" name="Total Time (hours)" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[Total Time (min)]]/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0D881C58-476D-4010-A5E7-8B9017364742}" name="Total Time (days)" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{0D881C58-476D-4010-A5E7-8B9017364742}" name="Total Time (days)" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[Total Time (hours)]]/24</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{2CA2A291-742D-470A-9587-3BD82255574C}" name="Pros" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{C7B4DAED-86E8-45DC-916B-52EFF68BF89E}" name="Cons" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{C7B4DAED-86E8-45DC-916B-52EFF68BF89E}" name="Cons" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{3FCFBCCF-7C1E-4051-8852-0800C5C27E06}" name="Method_" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -659,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216D571E-86AD-4974-B919-982C7747BBD2}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,16 +695,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>709656969216</v>
+        <v>1260988713616.6899</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>44251</v>
+        <v>44262</v>
       </c>
       <c r="F3" t="str">
-        <f>VLOOKUP(MIN(A:A), A1:B7,2,FALSE)</f>
+        <f>VLOOKUP(MIN(A:A), A1:B5,2,FALSE)</f>
         <v>AWS - TFIDF</v>
       </c>
       <c r="G3" t="s">
@@ -716,79 +713,71 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>901931000878.56995</v>
+        <v>314380091392</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>44253</v>
+        <v>44255</v>
       </c>
       <c r="F4" s="4">
         <f>1-MIN(A:A)/MAX(A:A)</f>
         <v>0.83143319991760467</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>1283456106496</v>
+        <v>1040071490897.22</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>44253</v>
+        <v>44261</v>
       </c>
       <c r="F5" s="4">
-        <f>1-MIN(A:A)/A6</f>
-        <v>0.5969616625481492</v>
+        <f>1-MIN(A:A)/A3</f>
+        <v>0.75068762472083161</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>780025278437.82996</v>
+        <v>1125427766274.45</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
-        <v>44253</v>
+        <v>44262</v>
       </c>
       <c r="F6" s="4">
-        <f>1-A7/A6</f>
-        <v>0.5969616625481492</v>
+        <f>1-A4/A3</f>
+        <v>0.75068762472083161</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>314380091392</v>
+        <v>569715637462</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
-        <v>44255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>1695799635366.3501</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44256</v>
-      </c>
+        <v>44264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -801,7 +790,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A22"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,13 +809,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1">
         <v>60</v>
@@ -834,12 +823,12 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(MIN(Table1[Total Time (min)]),Table1[[#All],[Total Time (min)]:[Method_]],6, FALSE)</f>
@@ -854,12 +843,12 @@
         <v>0.99937001473352638</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(MAX(Table1[Total Time (min)]),Table1[[#All],[Total Time (min)]:[Method_]],6, FALSE)</f>
@@ -874,12 +863,12 @@
         <v>0.65555555555555556</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <f>VLOOKUP(B6,Table1[#All],4,FALSE)</f>
@@ -888,39 +877,39 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="F9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="J9" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="9">
         <f>3^9</f>
@@ -947,18 +936,18 @@
         <v>68.34375</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="9">
         <f>INT(B10*0.25)</f>
@@ -985,18 +974,18 @@
         <v>17.083333333333332</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="9">
         <v>60</v>
@@ -1021,18 +1010,18 @@
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" s="9">
         <v>36</v>
@@ -1058,13 +1047,13 @@
         <v>0.125</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Set pipeline to save imputer and scaler for later data transformations. Edited model object to include ETL on init
</commit_message>
<xml_diff>
--- a/docs/Model Histories.xlsx
+++ b/docs/Model Histories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\Real_Estate_Analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E021000-FF99-4CAE-8D01-BB03696FFE9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32F0160-5EB1-454A-8BF8-35710575D2AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11544" yWindow="2232" windowWidth="19176" windowHeight="11856" xr2:uid="{A6735569-3412-48D9-A81F-E34E4DFEE9CE}"/>
+    <workbookView xWindow="26364" yWindow="5148" windowWidth="19176" windowHeight="11856" xr2:uid="{A6735569-3412-48D9-A81F-E34E4DFEE9CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -659,7 +659,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,14 +767,17 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>569715637462</v>
+        <v>316701856734</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1">
-        <v>44264</v>
-      </c>
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>

</xml_diff>